<commit_message>
fixing 3000 files from BES
</commit_message>
<xml_diff>
--- a/database/sia/expdata/3000.xlsx
+++ b/database/sia/expdata/3000.xlsx
@@ -67,7 +67,7 @@
     <t>pi</t>
   </si>
   <si>
-    <t>AUL-0-PT</t>
+    <t>AUL-0-PT-INT</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>10.6</v>
+        <v>3.65</v>
       </c>
       <c r="B2">
         <v>0.589</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>10.6</v>
+        <v>3.65</v>
       </c>
       <c r="B3">
         <v>0.576</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>10.6</v>
+        <v>3.65</v>
       </c>
       <c r="B4">
         <v>0.572</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>10.6</v>
+        <v>3.65</v>
       </c>
       <c r="B5">
         <v>0.5629999999999999</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>10.6</v>
+        <v>3.65</v>
       </c>
       <c r="B6">
         <v>0.5639999999999999</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7">
-        <v>10.6</v>
+        <v>3.65</v>
       </c>
       <c r="B7">
         <v>0.57</v>

</xml_diff>

<commit_message>
Remove spaces from SIA files
</commit_message>
<xml_diff>
--- a/database/sia/expdata/3000.xlsx
+++ b/database/sia/expdata/3000.xlsx
@@ -86,7 +86,7 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="14"/>
@@ -188,7 +188,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -211,9 +211,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -283,14 +280,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office Theme">
       <a:majorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office Theme">
@@ -385,9 +382,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -467,7 +464,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -495,10 +492,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -754,9 +751,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1044,7 +1041,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1072,10 +1069,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1326,7 +1323,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1685,62 +1682,11 @@
         <v>112.36</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>